<commit_message>
Enables lastest gemini model and ensured web search is working! by modifying prompts
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>application_name</t>
   </si>
@@ -37,28 +37,46 @@
     <t>payment_details</t>
   </si>
   <si>
-    <t>Todoist</t>
-  </si>
-  <si>
-    <t>Task Management</t>
-  </si>
-  <si>
-    <t>Personal &amp; Team Task Management</t>
-  </si>
-  <si>
-    <t>No (No User Management API Access)</t>
+    <t>Synchroteam</t>
+  </si>
+  <si>
+    <t>Field Service Management</t>
+  </si>
+  <si>
+    <t>Scheduling &amp; Dispatching</t>
+  </si>
+  <si>
+    <t>Yes (14 days - Full) - 95%</t>
   </si>
   <si>
     <t>REST API</t>
   </si>
   <si>
-    <t>No (No /users, /roles, or permission-related endpoints documented)</t>
-  </si>
-  <si>
-    <t>https://todoist.com</t>
-  </si>
-  <si>
-    <t>N/A</t>
+    <t>Yes - /User/Send, /User/List</t>
+  </si>
+  <si>
+    <t>https://www.synchroteam.com</t>
+  </si>
+  <si>
+    <t>No credit card required</t>
+  </si>
+  <si>
+    <t>Yeastar</t>
+  </si>
+  <si>
+    <t>Unified Communications</t>
+  </si>
+  <si>
+    <t>Business Phone Systems (PBX)</t>
+  </si>
+  <si>
+    <t>Yes (30 days - Full) - 90%</t>
+  </si>
+  <si>
+    <t>Yes - /extensionlist/query, /extension/update</t>
+  </si>
+  <si>
+    <t>https://www.yeastar.com</t>
   </si>
 </sst>
 </file>
@@ -435,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -487,6 +505,32 @@
         <v>14</v>
       </c>
       <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>